<commit_message>
Speeded up the add/remove agent method of grid
</commit_message>
<xml_diff>
--- a/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
+++ b/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Dropbox\ABM4ALL\Melodie\examples\Covid\data\excel_source\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30240" windowHeight="13035"/>
+    <workbookView windowWidth="30240" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -48,31 +43,367 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -80,25 +411,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -356,25 +973,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="7.14285714285714" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="18.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -411,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -437,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -458,5 +1075,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the calibrator, removed the old calibrator.
</commit_message>
<xml_diff>
--- a/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
+++ b/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="14760"/>
+    <workbookView windowWidth="30240" windowHeight="12980"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -66,14 +66,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -81,12 +104,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -103,15 +166,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,90 +203,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -218,79 +218,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,103 +386,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,29 +412,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -454,17 +442,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,6 +473,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,159 +503,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -979,13 +979,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="14.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="7.14285714285714" customWidth="1"/>
@@ -1028,16 +1028,16 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>1000</v>
       </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
       <c r="E2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
@@ -1054,22 +1054,48 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>10000</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
       </c>
       <c r="H3" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the documentation, added the contribution.rst, but unfinished yet.
</commit_message>
<xml_diff>
--- a/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
+++ b/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
@@ -45,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -79,6 +79,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -87,9 +103,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -103,8 +125,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,14 +180,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,63 +202,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -224,55 +224,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,121 +392,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,32 +412,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -447,32 +426,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,159 +454,206 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -979,13 +979,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="14.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="7.14285714285714" customWidth="1"/>
@@ -1072,32 +1072,6 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
optimized the package layout of trainer and calibrator; optimized imports
</commit_message>
<xml_diff>
--- a/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
+++ b/examples/VirusContagion/data/excel_source/simulator_scenarios.xlsx
@@ -46,9 +46,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -66,24 +66,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -95,23 +102,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,37 +142,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,14 +151,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,7 +173,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,25 +224,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,19 +368,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,127 +380,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,6 +409,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -430,30 +439,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -465,6 +450,32 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -485,175 +496,164 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -982,7 +982,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="2" outlineLevelCol="7"/>

</xml_diff>